<commit_message>
Some basic plots for Jon
</commit_message>
<xml_diff>
--- a/data/S3 Raw Data.xlsx
+++ b/data/S3 Raw Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ssu-my.sharepoint.com/personal/jon_cooper_solent_ac_uk/Documents/PhD/S3 Longitudinal/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Dropbox\Research\Jon Cooper\IZOF_SnC\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3072" documentId="8_{9262A02C-B43B-48F6-8B5A-8277541935CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4D8DC1A-CFDB-42F5-A426-62794D5CB896}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{204F03D3-D41B-44DE-96E8-E6459ABC6C61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{02A6D00F-F217-4A79-9E70-F1470F541659}"/>
+    <workbookView xWindow="4950" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{02A6D00F-F217-4A79-9E70-F1470F541659}"/>
   </bookViews>
   <sheets>
     <sheet name="Demographic" sheetId="3" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="86">
   <si>
     <t>P+I</t>
   </si>
@@ -159,15 +159,6 @@
   </si>
   <si>
     <t>Endurance Rating</t>
-  </si>
-  <si>
-    <t>SRating</t>
-  </si>
-  <si>
-    <t>PRating</t>
-  </si>
-  <si>
-    <t>MERating</t>
   </si>
   <si>
     <t>FAthl1</t>
@@ -675,7 +666,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4991814-5480-499E-95CE-CE49E8D40013}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
@@ -706,7 +697,7 @@
         <v>31</v>
       </c>
       <c r="G1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H1" t="s">
         <v>33</v>
@@ -717,28 +708,28 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B2">
         <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E2">
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G2">
         <v>4</v>
       </c>
       <c r="H2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I2">
         <v>3</v>
@@ -746,28 +737,28 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B3">
         <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="1">
+        <v>2</v>
+      </c>
+      <c r="H3" t="s">
         <v>44</v>
-      </c>
-      <c r="E3">
-        <v>3</v>
-      </c>
-      <c r="F3" t="s">
-        <v>46</v>
-      </c>
-      <c r="G3" s="1">
-        <v>2</v>
-      </c>
-      <c r="H3" t="s">
-        <v>47</v>
       </c>
       <c r="I3">
         <v>3</v>
@@ -775,28 +766,28 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B4">
         <v>20</v>
       </c>
       <c r="C4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
         <v>43</v>
       </c>
-      <c r="D4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
-      <c r="F4" t="s">
-        <v>46</v>
-      </c>
       <c r="G4">
         <v>2</v>
       </c>
       <c r="H4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -804,28 +795,28 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B5">
         <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E5">
         <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G5">
         <v>7</v>
       </c>
       <c r="H5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I5">
         <v>1</v>
@@ -833,28 +824,28 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B6">
         <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E6">
         <v>13</v>
       </c>
       <c r="F6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G6">
         <v>13</v>
       </c>
       <c r="H6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -862,28 +853,28 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B7">
         <v>19</v>
       </c>
       <c r="C7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
         <v>43</v>
       </c>
-      <c r="D7" t="s">
-        <v>51</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7" t="s">
-        <v>46</v>
-      </c>
       <c r="G7">
         <v>1</v>
       </c>
       <c r="H7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I7">
         <v>1</v>
@@ -891,28 +882,28 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B8">
         <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E8">
         <v>12</v>
       </c>
       <c r="F8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G8">
         <v>2</v>
       </c>
       <c r="H8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I8">
         <v>2</v>
@@ -920,28 +911,28 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B9">
         <v>21</v>
       </c>
       <c r="C9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
         <v>43</v>
       </c>
-      <c r="D9" t="s">
-        <v>59</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9" t="s">
-        <v>46</v>
-      </c>
       <c r="G9">
         <v>1</v>
       </c>
       <c r="H9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I9">
         <v>1</v>
@@ -949,28 +940,28 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B10">
         <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D10" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E10">
         <v>12</v>
       </c>
       <c r="F10" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G10">
         <v>2</v>
       </c>
       <c r="H10" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I10">
         <v>2</v>
@@ -978,28 +969,28 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B11">
         <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D11" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E11">
         <v>7</v>
       </c>
       <c r="F11" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G11">
         <v>3</v>
       </c>
       <c r="H11" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I11">
         <v>5</v>
@@ -1007,28 +998,28 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B12">
         <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D12" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E12">
         <v>9</v>
       </c>
       <c r="F12" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G12">
         <v>5</v>
       </c>
       <c r="H12" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I12">
         <v>4</v>
@@ -1036,28 +1027,28 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B13">
         <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D13" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E13">
         <v>9</v>
       </c>
       <c r="F13" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G13">
         <v>2</v>
       </c>
       <c r="H13" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I13">
         <v>1</v>
@@ -1065,28 +1056,28 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B14">
         <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D14" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E14">
         <v>10</v>
       </c>
       <c r="F14" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G14">
         <v>5</v>
       </c>
       <c r="H14" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I14">
         <v>3</v>
@@ -1094,28 +1085,28 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B15">
         <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D15" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E15">
         <v>10</v>
       </c>
       <c r="F15" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G15">
         <v>4</v>
       </c>
       <c r="H15" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I15">
         <v>6</v>
@@ -1123,28 +1114,28 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B16">
         <v>22</v>
       </c>
       <c r="C16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16" t="s">
         <v>43</v>
       </c>
-      <c r="D16" t="s">
-        <v>56</v>
-      </c>
-      <c r="E16">
-        <v>2</v>
-      </c>
-      <c r="F16" t="s">
-        <v>46</v>
-      </c>
       <c r="G16">
         <v>2</v>
       </c>
       <c r="H16" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I16">
         <v>2</v>
@@ -1152,28 +1143,28 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B17">
         <v>20</v>
       </c>
       <c r="C17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17" t="s">
         <v>43</v>
       </c>
-      <c r="D17" t="s">
-        <v>64</v>
-      </c>
-      <c r="E17">
-        <v>2</v>
-      </c>
-      <c r="F17" t="s">
-        <v>46</v>
-      </c>
       <c r="G17">
         <v>1</v>
       </c>
       <c r="H17" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I17">
         <v>1</v>
@@ -1181,28 +1172,28 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B18">
         <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D18" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E18">
         <v>15</v>
       </c>
       <c r="F18" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G18">
         <v>8</v>
       </c>
       <c r="H18" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I18">
         <v>5</v>
@@ -1210,28 +1201,28 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B19">
         <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D19" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E19">
         <v>4</v>
       </c>
       <c r="F19" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G19">
         <v>4</v>
       </c>
       <c r="H19" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I19">
         <v>4</v>
@@ -1239,28 +1230,28 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B20">
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D20" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E20">
         <v>6</v>
       </c>
       <c r="F20" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G20">
         <v>5</v>
       </c>
       <c r="H20" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I20">
         <v>6</v>
@@ -1268,28 +1259,28 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B21">
         <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D21" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E21">
         <v>5</v>
       </c>
       <c r="F21" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G21">
         <v>5</v>
       </c>
       <c r="H21" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I21">
         <v>5</v>
@@ -1297,28 +1288,28 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B22">
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D22" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E22">
         <v>1</v>
       </c>
       <c r="F22" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G22">
         <v>1</v>
       </c>
       <c r="H22" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I22">
         <v>1</v>
@@ -1326,28 +1317,28 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B23">
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D23" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E23">
         <v>1</v>
       </c>
       <c r="F23" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G23">
         <v>1</v>
       </c>
       <c r="H23" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I23">
         <v>1</v>
@@ -1355,28 +1346,28 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B24">
         <v>19</v>
       </c>
       <c r="C24" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D24" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E24">
         <v>7</v>
       </c>
       <c r="F24" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G24">
         <v>5</v>
       </c>
       <c r="H24" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I24">
         <v>2</v>
@@ -1384,28 +1375,28 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B25">
         <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D25" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E25">
         <v>6</v>
       </c>
       <c r="F25" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G25">
         <v>3</v>
       </c>
       <c r="H25" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I25">
         <v>6</v>
@@ -1413,28 +1404,28 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B26">
         <v>22</v>
       </c>
       <c r="C26" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D26" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E26">
         <v>9</v>
       </c>
       <c r="F26" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G26">
         <v>4</v>
       </c>
       <c r="H26" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I26">
         <v>6</v>
@@ -1442,28 +1433,28 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B27">
         <v>23</v>
       </c>
       <c r="C27" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D27" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E27">
         <v>14</v>
       </c>
       <c r="F27" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G27">
         <v>1</v>
       </c>
       <c r="H27" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I27">
         <v>8</v>
@@ -1471,28 +1462,28 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B28">
         <v>20</v>
       </c>
       <c r="C28" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D28" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E28">
         <v>1</v>
       </c>
       <c r="F28" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G28">
         <v>1</v>
       </c>
       <c r="H28" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I28">
         <v>1</v>
@@ -1500,28 +1491,28 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B29">
         <v>22</v>
       </c>
       <c r="C29" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D29" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E29">
         <v>14</v>
       </c>
       <c r="F29" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G29">
         <v>5</v>
       </c>
       <c r="H29" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I29">
         <v>7</v>
@@ -1529,28 +1520,28 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B30">
         <v>25</v>
       </c>
       <c r="C30" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D30" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E30">
         <v>10</v>
       </c>
       <c r="F30" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G30">
         <v>3</v>
       </c>
       <c r="H30" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I30">
         <v>2</v>
@@ -1558,28 +1549,28 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B31">
         <v>19</v>
       </c>
       <c r="C31" t="s">
+        <v>40</v>
+      </c>
+      <c r="D31" t="s">
+        <v>78</v>
+      </c>
+      <c r="E31">
+        <v>2</v>
+      </c>
+      <c r="F31" t="s">
         <v>43</v>
       </c>
-      <c r="D31" t="s">
-        <v>81</v>
-      </c>
-      <c r="E31">
-        <v>2</v>
-      </c>
-      <c r="F31" t="s">
-        <v>46</v>
-      </c>
       <c r="G31">
         <v>1</v>
       </c>
       <c r="H31" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I31">
         <v>1</v>
@@ -1587,28 +1578,28 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B32">
         <v>25</v>
       </c>
       <c r="C32" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D32" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E32">
         <v>17</v>
       </c>
       <c r="F32" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G32">
         <v>10</v>
       </c>
       <c r="H32" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I32">
         <v>6</v>
@@ -1616,28 +1607,28 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B33">
         <v>26</v>
       </c>
       <c r="C33" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D33" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E33">
         <v>15</v>
       </c>
       <c r="F33" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G33">
         <v>5</v>
       </c>
       <c r="H33" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I33">
         <v>6</v>
@@ -1653,8 +1644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{093A95AD-66A2-4BDE-93EF-EF5CF14D65B1}">
   <dimension ref="A1:AF33"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AG33" sqref="AG33"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AD1" sqref="AD1:AF1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1754,18 +1745,18 @@
         <v>26</v>
       </c>
       <c r="AD1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="AE1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="AF1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B2">
         <v>3</v>
@@ -1863,7 +1854,7 @@
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -1961,7 +1952,7 @@
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -2059,7 +2050,7 @@
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -2157,7 +2148,7 @@
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B6">
         <v>3</v>
@@ -2255,7 +2246,7 @@
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B7">
         <v>3</v>
@@ -2353,7 +2344,7 @@
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -2451,7 +2442,7 @@
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -2549,7 +2540,7 @@
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B10">
         <v>3</v>
@@ -2647,7 +2638,7 @@
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -2745,7 +2736,7 @@
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B12">
         <v>4</v>
@@ -2843,7 +2834,7 @@
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -2941,7 +2932,7 @@
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B14">
         <v>3</v>
@@ -3039,7 +3030,7 @@
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B15">
         <v>3</v>
@@ -3137,7 +3128,7 @@
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B16">
         <v>3</v>
@@ -3235,7 +3226,7 @@
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B17">
         <v>2</v>
@@ -3333,7 +3324,7 @@
     </row>
     <row r="18" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B18">
         <v>4</v>
@@ -3431,7 +3422,7 @@
     </row>
     <row r="19" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B19">
         <v>3</v>
@@ -3529,7 +3520,7 @@
     </row>
     <row r="20" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B20">
         <v>3</v>
@@ -3627,7 +3618,7 @@
     </row>
     <row r="21" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B21">
         <v>3</v>
@@ -3725,7 +3716,7 @@
     </row>
     <row r="22" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B22">
         <v>3</v>
@@ -3823,7 +3814,7 @@
     </row>
     <row r="23" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B23">
         <v>3</v>
@@ -3921,7 +3912,7 @@
     </row>
     <row r="24" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B24">
         <v>3</v>
@@ -4019,7 +4010,7 @@
     </row>
     <row r="25" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -4117,7 +4108,7 @@
     </row>
     <row r="26" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -4215,7 +4206,7 @@
     </row>
     <row r="27" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -4313,7 +4304,7 @@
     </row>
     <row r="28" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B28">
         <v>4</v>
@@ -4411,7 +4402,7 @@
     </row>
     <row r="29" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B29">
         <v>2</v>
@@ -4509,7 +4500,7 @@
     </row>
     <row r="30" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -4607,7 +4598,7 @@
     </row>
     <row r="31" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B31">
         <v>3</v>
@@ -4705,7 +4696,7 @@
     </row>
     <row r="32" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B32">
         <v>3</v>
@@ -4803,7 +4794,7 @@
     </row>
     <row r="33" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B33">
         <v>2</v>
@@ -4910,7 +4901,7 @@
   <dimension ref="A1:AF32"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AG32" sqref="AG32"/>
+      <selection activeCell="AD1" sqref="AD1:AF1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5015,7 +5006,7 @@
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -5113,7 +5104,7 @@
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -5211,27 +5202,27 @@
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -5329,12 +5320,12 @@
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -5432,12 +5423,12 @@
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B12">
         <v>3</v>
@@ -5535,7 +5526,7 @@
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B13">
         <v>3</v>
@@ -5633,7 +5624,7 @@
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B14">
         <v>3</v>
@@ -5731,7 +5722,7 @@
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B15">
         <v>3</v>
@@ -5829,7 +5820,7 @@
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -5927,7 +5918,7 @@
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B17">
         <v>3</v>
@@ -6025,7 +6016,7 @@
     </row>
     <row r="18" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B18">
         <v>3</v>
@@ -6123,7 +6114,7 @@
     </row>
     <row r="19" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B19">
         <v>2</v>
@@ -6221,7 +6212,7 @@
     </row>
     <row r="20" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B20">
         <v>3</v>
@@ -6319,7 +6310,7 @@
     </row>
     <row r="21" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B21">
         <v>2</v>
@@ -6417,7 +6408,7 @@
     </row>
     <row r="22" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -6515,12 +6506,12 @@
     </row>
     <row r="23" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B24">
         <v>4</v>
@@ -6618,7 +6609,7 @@
     </row>
     <row r="25" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -6716,7 +6707,7 @@
     </row>
     <row r="26" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -6814,12 +6805,12 @@
     </row>
     <row r="27" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="28" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B28">
         <v>3</v>
@@ -6917,12 +6908,12 @@
     </row>
     <row r="29" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="30" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B30">
         <v>2</v>
@@ -7020,7 +7011,7 @@
     </row>
     <row r="31" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B31">
         <v>2</v>
@@ -7118,7 +7109,7 @@
     </row>
     <row r="32" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B32">
         <v>3</v>
@@ -7333,7 +7324,7 @@
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B2">
         <v>3</v>
@@ -7431,7 +7422,7 @@
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -7529,47 +7520,47 @@
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B12">
         <v>3</v>
@@ -7667,7 +7658,7 @@
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -7765,17 +7756,17 @@
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B16">
         <v>3</v>
@@ -7873,7 +7864,7 @@
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -7971,7 +7962,7 @@
     </row>
     <row r="18" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B18">
         <v>3</v>
@@ -8069,7 +8060,7 @@
     </row>
     <row r="19" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B19">
         <v>2</v>
@@ -8167,7 +8158,7 @@
     </row>
     <row r="20" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B20">
         <v>3</v>
@@ -8265,7 +8256,7 @@
     </row>
     <row r="21" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B21">
         <v>2</v>
@@ -8363,22 +8354,22 @@
     </row>
     <row r="22" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -8476,37 +8467,37 @@
     </row>
     <row r="26" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="28" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="30" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="31" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="32" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B32">
         <v>3</v>
@@ -8720,7 +8711,7 @@
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B2">
         <v>3</v>
@@ -8818,7 +8809,7 @@
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -8916,77 +8907,77 @@
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -9084,37 +9075,37 @@
     </row>
     <row r="19" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B25">
         <v>3</v>
@@ -9212,37 +9203,37 @@
     </row>
     <row r="26" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="28" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="30" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="31" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="32" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B32">
         <v>3</v>
@@ -9459,7 +9450,7 @@
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B2">
         <v>3</v>
@@ -9557,7 +9548,7 @@
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -9655,77 +9646,77 @@
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -9823,37 +9814,37 @@
     </row>
     <row r="19" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -9951,37 +9942,37 @@
     </row>
     <row r="26" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="28" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="30" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="31" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="32" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B32">
         <v>2</v>
@@ -10192,7 +10183,7 @@
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B2">
         <v>4</v>
@@ -10290,7 +10281,7 @@
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -10388,77 +10379,77 @@
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B18">
         <v>3</v>
@@ -10556,37 +10547,37 @@
     </row>
     <row r="19" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -10684,37 +10675,37 @@
     </row>
     <row r="26" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="28" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="30" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="31" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="32" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B32">
         <v>3</v>

</xml_diff>